<commit_message>
Started working on the draft analysis doc
</commit_message>
<xml_diff>
--- a/output/analysis/session_consistency_06212020/Async point read vs async partition key read RU comparison .xlsx
+++ b/output/analysis/session_consistency_06212020/Async point read vs async partition key read RU comparison .xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/deepu/projects/CosmosSQLCalipers/output/analysis/session_consistency_06212020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA92F3F-BA79-2942-82DE-C9D591AEA186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C101A874-85E8-0541-8825-5C836F57E6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{A1A989E4-1668-6E45-97AA-EDE886FADC77}"/>
   </bookViews>
@@ -1764,6 +1764,390 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Async point reads vs async partition key reads RU comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>async_point_read_1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>async_point_read_5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>async_point_read_10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>async_point_read_50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>async_point_read_100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>async_point_read_200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>async_point_read_400k</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>async_partition_read_1k</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>async_partition_read_5k</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>async_partition_read_10k</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>async_partition_read_50k</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>async_partition_read_100k</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>async_partition_read_200k</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>async_partition_read_400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5DC0-8547-8F4C-D60A96E12FEB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="990427631"/>
+        <c:axId val="990422799"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="990427631"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990422799"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="990422799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="990427631"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1804,7 +2188,550 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2340,6 +3267,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1962150</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E41F386E-5763-DC42-91FA-79F8213816F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2647,8 +3610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C03D4E5-7BAB-EE46-92AB-7A3C1EA2EC16}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="Y22" sqref="Y22"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated the main README to provide a link to the latest tests
</commit_message>
<xml_diff>
--- a/output/analysis/session_consistency_06212020/Async point read vs async partition key read RU comparison .xlsx
+++ b/output/analysis/session_consistency_06212020/Async point read vs async partition key read RU comparison .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/deepu/projects/CosmosSQLCalipers/output/analysis/session_consistency_06212020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C101A874-85E8-0541-8825-5C836F57E6F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BA4A38-D3C2-8A4B-AA2C-2AD6D3E8A1DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" xr2:uid="{A1A989E4-1668-6E45-97AA-EDE886FADC77}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>payload</t>
   </si>
@@ -108,6 +108,36 @@
   </si>
   <si>
     <t>async_partition_read_400k</t>
+  </si>
+  <si>
+    <t>operation</t>
+  </si>
+  <si>
+    <t>Doc size 1k</t>
+  </si>
+  <si>
+    <t>Doc size 5k</t>
+  </si>
+  <si>
+    <t>Doc size 10k</t>
+  </si>
+  <si>
+    <t>Doc size 50k</t>
+  </si>
+  <si>
+    <t>Doc size 100k</t>
+  </si>
+  <si>
+    <t>Doc size 200k</t>
+  </si>
+  <si>
+    <t>Doc size 400k</t>
+  </si>
+  <si>
+    <t>point read</t>
+  </si>
+  <si>
+    <t>partition key SELECT</t>
   </si>
 </sst>
 </file>
@@ -2148,6 +2178,463 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2000" b="1" baseline="0"/>
+              <a:t>Point read vs partition key based operations</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>point read</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$1:$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Doc size 1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Doc size 5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Doc size 10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Doc size 50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Doc size 100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Doc size 200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Doc size 400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$2:$Y$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D4DE-4948-9857-C69F1034E2D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>partition key SELECT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$S$1:$Y$1</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Doc size 1k</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Doc size 5k</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Doc size 10k</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Doc size 50k</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Doc size 100k</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Doc size 200k</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Doc size 400k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$3:$Y$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D4DE-4948-9857-C69F1034E2D5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2024754896"/>
+        <c:axId val="2024708560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2024754896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2024708560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2024708560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2024754896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2228,6 +2715,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2732,6 +3259,509 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3303,6 +4333,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>971550</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3B0512A-26D5-E84F-8F77-F58745F7778D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3608,18 +4674,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C03D4E5-7BAB-EE46-92AB-7A3C1EA2EC16}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="18" max="18" width="25.5" customWidth="1"/>
+    <col min="24" max="24" width="12.6640625" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3653,8 +4722,32 @@
       <c r="K1" t="s">
         <v>17</v>
       </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" t="s">
+        <v>28</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>30</v>
+      </c>
+      <c r="X1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -3688,8 +4781,32 @@
       <c r="K2">
         <v>1</v>
       </c>
+      <c r="R2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+      <c r="U2">
+        <v>2</v>
+      </c>
+      <c r="V2">
+        <v>5</v>
+      </c>
+      <c r="W2">
+        <v>10</v>
+      </c>
+      <c r="X2">
+        <v>20</v>
+      </c>
+      <c r="Y2">
+        <v>41</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -3723,8 +4840,32 @@
       <c r="K3">
         <v>1</v>
       </c>
+      <c r="R3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>3</v>
+      </c>
+      <c r="U3">
+        <v>3</v>
+      </c>
+      <c r="V3">
+        <v>4</v>
+      </c>
+      <c r="W3">
+        <v>7</v>
+      </c>
+      <c r="X3">
+        <v>10</v>
+      </c>
+      <c r="Y3">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -3759,7 +4900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -3794,7 +4935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -3829,7 +4970,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -3864,7 +5005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -3899,7 +5040,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -3934,7 +5075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -3969,7 +5110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4004,7 +5145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -4039,7 +5180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -4074,7 +5215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -4109,7 +5250,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -4146,6 +5287,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>